<commit_message>
updated bottom assembly layer and output files
</commit_message>
<xml_diff>
--- a/_schematics/Project Outputs for EEG_circuit/BOM/Bill of Materials-EEG_circuit.xlsx
+++ b/_schematics/Project Outputs for EEG_circuit/BOM/Bill of Materials-EEG_circuit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B30717F-C580-452C-A347-C429DB195B97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6148270F-7AA4-4D1D-8CA3-BF6F817FFF98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -125,7 +125,7 @@
     <t>2020-02-11</t>
   </si>
   <si>
-    <t>8:45:23 AM</t>
+    <t>1:42:53 PM</t>
   </si>
   <si>
     <t>Bill of Materials For Project [EEG_circuit.PrjPcb] (No PCB Document Selected)</t>
@@ -434,13 +434,13 @@
     <t>Supplier Currency 1</t>
   </si>
   <si>
-    <t>C:\Users\Public\Documents\Altium\Projects\EEG_circuit\EEG_circuit\Group49\_schematics\EEG_circuit.PrjPcb</t>
+    <t>C:\Users\dmerl\Documents\4th Year\ELEC491\repo\Group49\_schematics\EEG_circuit.PrjPcb</t>
   </si>
   <si>
     <t>60</t>
   </si>
   <si>
-    <t>2020-02-11 8:45:23 AM</t>
+    <t>2020-02-11 1:42:53 PM</t>
   </si>
   <si>
     <t>Bill of Materials</t>
@@ -2145,27 +2145,27 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="31" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="73" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" style="73" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.54296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.54296875" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="1"/>
+    <col min="15" max="15" width="8.26953125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="49"/>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -2203,7 +2203,7 @@
       <c r="N2" s="12"/>
       <c r="O2" s="60"/>
     </row>
-    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="52"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
@@ -2228,7 +2228,7 @@
       <c r="N3" s="36"/>
       <c r="O3" s="61"/>
     </row>
-    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="52"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
@@ -2276,7 +2276,7 @@
       <c r="N5" s="36"/>
       <c r="O5" s="61"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="52"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>43872.365029398148</v>
+        <v>43872.571857986113</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="20"/>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="O28" s="62"/>
     </row>
-    <row r="29" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="52"/>
       <c r="B29" s="77" t="s">
         <v>20</v>
@@ -3249,7 +3249,7 @@
       <c r="N29" s="36"/>
       <c r="O29" s="61"/>
     </row>
-    <row r="30" spans="1:15" ht="25.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="52"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="O31" s="61"/>
     </row>
-    <row r="32" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="55"/>
       <c r="B32" s="27"/>
       <c r="C32" s="11"/>
@@ -3512,60 +3512,60 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D10" r:id="rId2" tooltip="Component" display="'JST" xr:uid="{94807658-BFA0-4368-9F3C-257E47FD46C3}"/>
-    <hyperlink ref="D11" r:id="rId3" tooltip="Component" display="'Global Connector Technology" xr:uid="{FCF2EDD6-4E7C-4EB0-A31B-290113ABD387}"/>
-    <hyperlink ref="D12" r:id="rId4" tooltip="Component" display="'Wurth Electronics" xr:uid="{C13E1788-E266-4B55-A7E6-CFB78EE7519E}"/>
-    <hyperlink ref="D13" r:id="rId5" tooltip="Component" display="'Wurth Electronics" xr:uid="{07C294A8-0742-4F6A-98A0-975AD3AF75CD}"/>
-    <hyperlink ref="D14" r:id="rId6" tooltip="Component" display="'Wurth Electronics" xr:uid="{ECAE8289-1DEA-47EF-9583-750B5C3B5E0D}"/>
-    <hyperlink ref="D15" r:id="rId7" tooltip="Component" display="'Panasonic" xr:uid="{0D93523F-C1D1-4D4D-9C71-13EF2C87BD59}"/>
-    <hyperlink ref="D16" r:id="rId8" tooltip="Component" display="'Yageo" xr:uid="{80FC095A-EDEF-4A2B-B97E-F91A8AFE4606}"/>
-    <hyperlink ref="D17" r:id="rId9" tooltip="Component" display="'Murata, Samsung, KEMET" xr:uid="{3E1FAFC2-36F1-455F-9444-03A9963A2CD5}"/>
-    <hyperlink ref="D18" r:id="rId10" tooltip="Component" display="'TDK" xr:uid="{8F6855AB-DEC7-47D8-8FB0-8317FAD4FC1B}"/>
-    <hyperlink ref="D19" r:id="rId11" tooltip="Component" display="'Vishay Lite-On" xr:uid="{E54373CF-30E1-4AFC-84BA-1F59C1EFF583}"/>
-    <hyperlink ref="D20" r:id="rId12" tooltip="Component" display="'Yageo" xr:uid="{61CDD703-7298-4740-97E3-292E3E4DAFFD}"/>
-    <hyperlink ref="D21" r:id="rId13" tooltip="Component" display="'ECS International" xr:uid="{154CDB13-D3B2-400E-9F0A-263313D98371}"/>
-    <hyperlink ref="D22" r:id="rId14" tooltip="Component" display="'ITT C&amp;K" xr:uid="{D88D9677-500A-47F2-B2A3-4FD4AA91107A}"/>
-    <hyperlink ref="D23" r:id="rId15" tooltip="Component" display="'Diodes" xr:uid="{3EAFEBC5-DB13-434F-A7D4-0FCA256095CE}"/>
-    <hyperlink ref="D24" r:id="rId16" tooltip="Component" display="'Microchip" xr:uid="{8C39FD1A-D8A2-479A-9A83-5DE94565E7B3}"/>
-    <hyperlink ref="D25" r:id="rId17" tooltip="Component" display="'Vishay Semiconductors" xr:uid="{65901704-EB07-4AC4-BBBC-BE5639374B48}"/>
-    <hyperlink ref="D26" r:id="rId18" tooltip="Component" display="'Texas Instruments" xr:uid="{A7F2E39E-43ED-4C3E-8578-3299A32BD6D4}"/>
-    <hyperlink ref="D27" r:id="rId19" tooltip="Component" display="'Texas Instruments" xr:uid="{4E84FB60-97A1-4926-A272-1097F93EA105}"/>
-    <hyperlink ref="E10" r:id="rId20" tooltip="Manufacturer" display="'B2B-PH-SM4-TBT(LF)(SN)" xr:uid="{656B85E8-AD24-42CD-88B9-47085A2F84E1}"/>
-    <hyperlink ref="E11" r:id="rId21" tooltip="Manufacturer" display="'MEM2067-02-180-00-A" xr:uid="{407D36C2-84F6-4F6F-B864-A5B41F3C021D}"/>
-    <hyperlink ref="E12" r:id="rId22" tooltip="Manufacturer" display="'450404015514" xr:uid="{7586FAC5-4A0A-4D39-A836-E6E742E0B9B2}"/>
-    <hyperlink ref="E13" r:id="rId23" tooltip="Manufacturer" display="'61300621121" xr:uid="{1D51899B-66A4-4A8D-91DC-FF4DA38839C1}"/>
-    <hyperlink ref="E14" r:id="rId24" tooltip="Manufacturer" display="'61301211121" xr:uid="{F36C3002-C3AD-4855-BCE8-23AA3169D31E}"/>
-    <hyperlink ref="E15" r:id="rId25" tooltip="Manufacturer" display="'EXB-N8V162JX" xr:uid="{4A4EBBDD-13ED-4C62-A47C-9D29E91CCAF2}"/>
-    <hyperlink ref="E16" r:id="rId26" tooltip="Manufacturer" display="'RC0402FR-071ML, RC0402JR-070RL, RC0402FR-07453KL, RC0402FR-07100KL, RC0402JR-071M6L, RC0402JR-07180KL, RC0402FR-0710KL, RC0402FR-071KL, RC0402JR-07470KL" xr:uid="{AD9A7706-5D20-47F2-9722-8C8479E859B5}"/>
-    <hyperlink ref="E17" r:id="rId27" tooltip="Manufacturer" display="'GRM153R61A105ME95D, CL05A104KP5NNNC, CL05B152KB5NNNC, GRM155R61A475MEAAD, CL05A106MP5NUNC, GRM31CR60J107ME39L, C0402C180K5RAC7867" xr:uid="{FECA9DFE-B076-4B7B-A603-440BA29D3CED}"/>
-    <hyperlink ref="E18" r:id="rId28" tooltip="Manufacturer" display="'MLZ1608A2R2WT000, MLZ1608M4R7WT000" xr:uid="{1B1F8E71-D0DA-47D8-A9D5-F3CB49F07D75}"/>
-    <hyperlink ref="E19" r:id="rId29" tooltip="Manufacturer" display="'LTST-C193TBKT-5A" xr:uid="{1576B5EA-84D9-40A8-86A8-666C41C77CD4}"/>
-    <hyperlink ref="E20" r:id="rId30" tooltip="Manufacturer" display="'CA0612KRX7R9BB102" xr:uid="{890E9033-4FC0-47CC-B684-E1DFAC61EE1F}"/>
-    <hyperlink ref="E21" r:id="rId31" tooltip="Manufacturer" display="'ECS-80-18-30-JGN-TR" xr:uid="{43217FD5-8EC5-47A3-B083-7AD130B2B672}"/>
-    <hyperlink ref="E22" r:id="rId32" tooltip="Manufacturer" display="'PTS810SJK250SMTRLFS" xr:uid="{64E3F94D-A75B-43DE-8F23-988C7CCC232A}"/>
-    <hyperlink ref="E23" r:id="rId33" tooltip="Manufacturer" display="'AP3417CKTR-G1" xr:uid="{81093F81-38D5-4AA3-BD6C-212A63EB2E34}"/>
-    <hyperlink ref="E24" r:id="rId34" tooltip="Manufacturer" display="'PIC32MX250F128B-I/SS" xr:uid="{E0BDC278-9999-43BA-965E-FB27626DBD1A}"/>
-    <hyperlink ref="E25" r:id="rId35" tooltip="Manufacturer" display="'GSOT04C-G3-08" xr:uid="{EC45D2F3-34E3-4E4D-92F4-9DDB4F390CFC}"/>
-    <hyperlink ref="E26" r:id="rId36" tooltip="Manufacturer" display="'ADS1299IPAGR" xr:uid="{D1D0F11A-4830-43B3-92FB-CF5780ABBC27}"/>
-    <hyperlink ref="E27" r:id="rId37" tooltip="Manufacturer" display="'TPS61073DDCR" xr:uid="{480BFBBB-8A7E-4F03-A3AA-8D7058566DB8}"/>
-    <hyperlink ref="J10" r:id="rId38" tooltip="Supplier" display="'455-2872-6-ND" xr:uid="{BABB3C35-836D-4A41-8256-8FBCD49A620E}"/>
-    <hyperlink ref="J11" r:id="rId39" tooltip="Supplier" display="'2073-MEM2067-02-180-00-ACT-ND" xr:uid="{8C5B88E2-AF1C-4BD8-9188-D4115AD53345}"/>
-    <hyperlink ref="J12" r:id="rId40" tooltip="Supplier" display="'732-13665-6-ND" xr:uid="{85FE3E9A-EE3A-4F5A-A422-19B36523F8A4}"/>
-    <hyperlink ref="J13" r:id="rId41" tooltip="Supplier" display="'732-5295-ND" xr:uid="{98840115-5A68-47DB-A367-E8A0166962AD}"/>
-    <hyperlink ref="J14" r:id="rId42" tooltip="Supplier" display="'732-5323-ND" xr:uid="{C88ECFE9-A204-4BC2-AAA4-D3D7B5158D98}"/>
-    <hyperlink ref="J15" r:id="rId43" tooltip="Supplier" display="'Y10162DKR-ND" xr:uid="{AD587701-53A7-4A8D-B4DC-E021216837E5}"/>
-    <hyperlink ref="J16" r:id="rId44" tooltip="Supplier" display="'311-1.00MLRCT-ND, 311-0.0JRDKR-ND, YAG3164DKR-ND, 311-100KLRCT-ND, YAG3284DKR-ND, 311-180KJRDKR-ND, 311-10.0KLRDKR-ND, 311-1.00KLRDKR-ND, 311-470KJRDKR-ND" xr:uid="{8A6323A5-0E5D-4B94-8C8E-E767083141ED}"/>
-    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'490-14577-6-ND, 1276-1022-6-ND, 1276-1521-6-ND, 490-14306-6-ND, 1276-1450-6-ND, 490-4539-6-ND, 399-19371-6-ND" xr:uid="{ADA0337B-3247-479D-AFE3-9074C37171DD}"/>
-    <hyperlink ref="J18" r:id="rId46" tooltip="Supplier" display="'445-6385-6-ND, 445-6390-6-ND" xr:uid="{00C2EB9F-C310-4814-AC65-450BC4CCF352}"/>
-    <hyperlink ref="J19" r:id="rId47" tooltip="Supplier" display="'160-1827-1-ND" xr:uid="{84E446E0-B19C-4126-9CCF-2A6B4853C616}"/>
-    <hyperlink ref="J20" r:id="rId48" tooltip="Supplier" display="'311-2073-6-ND" xr:uid="{B35093E6-91B3-4536-BDD1-9A63A002598C}"/>
-    <hyperlink ref="J21" r:id="rId49" tooltip="Supplier" display="'XC2103DKR-ND" xr:uid="{165A2CF2-4F8B-432A-9738-DEB35F0A89A6}"/>
-    <hyperlink ref="J22" r:id="rId50" tooltip="Supplier" display="'CKN10503DKR-ND" xr:uid="{042D0870-19E1-4458-A91D-17DCE210616E}"/>
-    <hyperlink ref="J23" r:id="rId51" tooltip="Supplier" display="'AP3417CKTR-G1DIDKR-ND" xr:uid="{8C9CB2FC-F551-4DF9-995C-25C862EBFB43}"/>
-    <hyperlink ref="J24" r:id="rId52" tooltip="Supplier" display="'PIC32MX250F128B-I/SS-ND" xr:uid="{8A81D2F5-CD9D-489A-BF65-15C962C841FB}"/>
-    <hyperlink ref="J25" r:id="rId53" tooltip="Supplier" display="'GSOT04C-G3-08GIDKR-ND" xr:uid="{DD1AA63E-8036-4E42-985E-F701872B293A}"/>
-    <hyperlink ref="J26" r:id="rId54" tooltip="Supplier" display="'296-34818-6-ND" xr:uid="{A2572D68-B727-48FD-B3FB-20FF874647D1}"/>
-    <hyperlink ref="J27" r:id="rId55" tooltip="Supplier" display="'296-21898-2-ND" xr:uid="{39B2CF25-0814-4268-800C-3442D154E8AC}"/>
+    <hyperlink ref="D10" r:id="rId2" tooltip="Component" display="'JST" xr:uid="{E17CCF0C-CA77-4AF2-AC5B-80A8951316D4}"/>
+    <hyperlink ref="D11" r:id="rId3" tooltip="Component" display="'Global Connector Technology" xr:uid="{8AD69FE7-D361-4A06-8B5D-58220CAE4C48}"/>
+    <hyperlink ref="D12" r:id="rId4" tooltip="Component" display="'Wurth Electronics" xr:uid="{821447E0-395D-447C-B3F0-786D1C72C06C}"/>
+    <hyperlink ref="D13" r:id="rId5" tooltip="Component" display="'Wurth Electronics" xr:uid="{F0F42E58-5414-4872-8D42-CDABAEF31BAF}"/>
+    <hyperlink ref="D14" r:id="rId6" tooltip="Component" display="'Wurth Electronics" xr:uid="{16D82F29-F51E-4BCE-A73E-D291925847FB}"/>
+    <hyperlink ref="D15" r:id="rId7" tooltip="Component" display="'Panasonic" xr:uid="{994E6F34-49CE-4442-9B91-844E590CCE3F}"/>
+    <hyperlink ref="D16" r:id="rId8" tooltip="Component" display="'Yageo" xr:uid="{9EEA62B6-FD2C-4591-8DB8-B9AC15816F20}"/>
+    <hyperlink ref="D17" r:id="rId9" tooltip="Component" display="'Murata, Samsung, KEMET" xr:uid="{AC4D51EB-6330-47A9-85E2-F2C866DD3B46}"/>
+    <hyperlink ref="D18" r:id="rId10" tooltip="Component" display="'TDK" xr:uid="{E93501FA-C544-465E-8376-435256E848E3}"/>
+    <hyperlink ref="D19" r:id="rId11" tooltip="Component" display="'Vishay Lite-On" xr:uid="{7A671E01-2B06-4F3E-B243-47F2A70C2282}"/>
+    <hyperlink ref="D20" r:id="rId12" tooltip="Component" display="'Yageo" xr:uid="{2364ED70-3793-4940-B3A6-E9380E02ECED}"/>
+    <hyperlink ref="D21" r:id="rId13" tooltip="Component" display="'ECS International" xr:uid="{6027C9AA-A15B-4F31-A5BE-A3C38C5CDF6B}"/>
+    <hyperlink ref="D22" r:id="rId14" tooltip="Component" display="'ITT C&amp;K" xr:uid="{802C777E-E8C0-4B9B-99A5-B9C133ABF11E}"/>
+    <hyperlink ref="D23" r:id="rId15" tooltip="Component" display="'Diodes" xr:uid="{E681CCC8-B3B8-4E5B-9052-DA8AB41B9FB8}"/>
+    <hyperlink ref="D24" r:id="rId16" tooltip="Component" display="'Microchip" xr:uid="{EB27A58A-2076-4830-8122-635583F22CDC}"/>
+    <hyperlink ref="D25" r:id="rId17" tooltip="Component" display="'Vishay Semiconductors" xr:uid="{8CBE7A95-84B7-4B4C-8980-FFBA63433157}"/>
+    <hyperlink ref="D26" r:id="rId18" tooltip="Component" display="'Texas Instruments" xr:uid="{3EDBDE57-5D16-4116-B073-CAB1D5E12CE3}"/>
+    <hyperlink ref="D27" r:id="rId19" tooltip="Component" display="'Texas Instruments" xr:uid="{AB61C659-5E4A-4E7F-8091-A0C1C8A98685}"/>
+    <hyperlink ref="E10" r:id="rId20" tooltip="Manufacturer" display="'B2B-PH-SM4-TBT(LF)(SN)" xr:uid="{C398540D-2562-4D55-8B25-69F89142FD02}"/>
+    <hyperlink ref="E11" r:id="rId21" tooltip="Manufacturer" display="'MEM2067-02-180-00-A" xr:uid="{05FF8958-9B7D-403C-89E7-831A1FF967FE}"/>
+    <hyperlink ref="E12" r:id="rId22" tooltip="Manufacturer" display="'450404015514" xr:uid="{C6AA90D6-775A-40A6-BF1C-2942D5E6BAC3}"/>
+    <hyperlink ref="E13" r:id="rId23" tooltip="Manufacturer" display="'61300621121" xr:uid="{E46A51EF-0CD3-4D0E-B11C-04CD6F3B27D7}"/>
+    <hyperlink ref="E14" r:id="rId24" tooltip="Manufacturer" display="'61301211121" xr:uid="{4126F58B-64EB-48E9-ADA3-53E87A432258}"/>
+    <hyperlink ref="E15" r:id="rId25" tooltip="Manufacturer" display="'EXB-N8V162JX" xr:uid="{851C9639-2AA7-4051-AD7C-9A846F6278FE}"/>
+    <hyperlink ref="E16" r:id="rId26" tooltip="Manufacturer" display="'RC0402FR-071ML, RC0402JR-070RL, RC0402FR-07453KL, RC0402FR-07100KL, RC0402JR-071M6L, RC0402JR-07180KL, RC0402FR-0710KL, RC0402FR-071KL, RC0402JR-07470KL" xr:uid="{66CFB7AA-0BAB-4440-9E47-2DE073582567}"/>
+    <hyperlink ref="E17" r:id="rId27" tooltip="Manufacturer" display="'GRM153R61A105ME95D, CL05A104KP5NNNC, CL05B152KB5NNNC, GRM155R61A475MEAAD, CL05A106MP5NUNC, GRM31CR60J107ME39L, C0402C180K5RAC7867" xr:uid="{7B70886D-5D47-4155-862F-114A40059966}"/>
+    <hyperlink ref="E18" r:id="rId28" tooltip="Manufacturer" display="'MLZ1608A2R2WT000, MLZ1608M4R7WT000" xr:uid="{DAAED366-F176-4783-8CFF-43FD9E11AA20}"/>
+    <hyperlink ref="E19" r:id="rId29" tooltip="Manufacturer" display="'LTST-C193TBKT-5A" xr:uid="{9DE918CC-D989-4B79-95F4-D12F6AC24A03}"/>
+    <hyperlink ref="E20" r:id="rId30" tooltip="Manufacturer" display="'CA0612KRX7R9BB102" xr:uid="{61B81365-FDA8-488A-87FC-0DCFE4CF8AAB}"/>
+    <hyperlink ref="E21" r:id="rId31" tooltip="Manufacturer" display="'ECS-80-18-30-JGN-TR" xr:uid="{ABD2BEFF-A50F-4DE1-9A40-C0E80D0D0B85}"/>
+    <hyperlink ref="E22" r:id="rId32" tooltip="Manufacturer" display="'PTS810SJK250SMTRLFS" xr:uid="{28CD9B91-DAAD-469F-9D31-2215DBBF2763}"/>
+    <hyperlink ref="E23" r:id="rId33" tooltip="Manufacturer" display="'AP3417CKTR-G1" xr:uid="{8AF274D8-87EE-46AB-8E52-0B9F7033901E}"/>
+    <hyperlink ref="E24" r:id="rId34" tooltip="Manufacturer" display="'PIC32MX250F128B-I/SS" xr:uid="{27C7DF5D-0D4A-4C31-ACA8-E4F4FC12EB99}"/>
+    <hyperlink ref="E25" r:id="rId35" tooltip="Manufacturer" display="'GSOT04C-G3-08" xr:uid="{490F205B-33CF-4390-896C-147AF756FE1E}"/>
+    <hyperlink ref="E26" r:id="rId36" tooltip="Manufacturer" display="'ADS1299IPAGR" xr:uid="{E1146058-33FF-4048-BCB6-4A64824CDCC4}"/>
+    <hyperlink ref="E27" r:id="rId37" tooltip="Manufacturer" display="'TPS61073DDCR" xr:uid="{39446364-C491-4226-B9C7-FD1CD60DE094}"/>
+    <hyperlink ref="J10" r:id="rId38" tooltip="Supplier" display="'455-2872-6-ND" xr:uid="{4D0A465C-FAA5-4639-A6E5-2630AFA5906F}"/>
+    <hyperlink ref="J11" r:id="rId39" tooltip="Supplier" display="'2073-MEM2067-02-180-00-ACT-ND" xr:uid="{CF1B3474-8070-409E-AE77-372DEBD666CB}"/>
+    <hyperlink ref="J12" r:id="rId40" tooltip="Supplier" display="'732-13665-6-ND" xr:uid="{62161FBE-5A25-4BD4-8BB8-838F78D0145A}"/>
+    <hyperlink ref="J13" r:id="rId41" tooltip="Supplier" display="'732-5295-ND" xr:uid="{8E9AF0C5-F08B-4DC0-8B33-58852FCD6F63}"/>
+    <hyperlink ref="J14" r:id="rId42" tooltip="Supplier" display="'732-5323-ND" xr:uid="{0232E260-FF16-49E6-94D2-3EE612F3884B}"/>
+    <hyperlink ref="J15" r:id="rId43" tooltip="Supplier" display="'Y10162DKR-ND" xr:uid="{319B4216-CE46-4571-80E9-4698BA7B9000}"/>
+    <hyperlink ref="J16" r:id="rId44" tooltip="Supplier" display="'311-1.00MLRCT-ND, 311-0.0JRDKR-ND, YAG3164DKR-ND, 311-100KLRCT-ND, YAG3284DKR-ND, 311-180KJRDKR-ND, 311-10.0KLRDKR-ND, 311-1.00KLRDKR-ND, 311-470KJRDKR-ND" xr:uid="{B12550CE-B39B-4151-8E94-17794D27192F}"/>
+    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'490-14577-6-ND, 1276-1022-6-ND, 1276-1521-6-ND, 490-14306-6-ND, 1276-1450-6-ND, 490-4539-6-ND, 399-19371-6-ND" xr:uid="{B24B7F2B-AA0F-4145-9CB6-E9ACCAE3E0B1}"/>
+    <hyperlink ref="J18" r:id="rId46" tooltip="Supplier" display="'445-6385-6-ND, 445-6390-6-ND" xr:uid="{35DAEC10-9C18-4104-B3F4-B91E10C36CB5}"/>
+    <hyperlink ref="J19" r:id="rId47" tooltip="Supplier" display="'160-1827-1-ND" xr:uid="{7881D3C6-51DB-42B0-AEAE-197FAB418104}"/>
+    <hyperlink ref="J20" r:id="rId48" tooltip="Supplier" display="'311-2073-6-ND" xr:uid="{F1F67F2D-CC8B-4549-BDC9-8527F20B7A32}"/>
+    <hyperlink ref="J21" r:id="rId49" tooltip="Supplier" display="'XC2103DKR-ND" xr:uid="{03A34192-D2AC-4C9A-A1E6-721BA70C6D50}"/>
+    <hyperlink ref="J22" r:id="rId50" tooltip="Supplier" display="'CKN10503DKR-ND" xr:uid="{D929463E-86F6-40C8-8D0F-114B511E46E4}"/>
+    <hyperlink ref="J23" r:id="rId51" tooltip="Supplier" display="'AP3417CKTR-G1DIDKR-ND" xr:uid="{98E19703-1CE9-4F9E-A3A3-5ADD5EC75BB6}"/>
+    <hyperlink ref="J24" r:id="rId52" tooltip="Supplier" display="'PIC32MX250F128B-I/SS-ND" xr:uid="{77972A37-6726-42E0-B48B-92AB90F2FFDA}"/>
+    <hyperlink ref="J25" r:id="rId53" tooltip="Supplier" display="'GSOT04C-G3-08GIDKR-ND" xr:uid="{B3E61186-8A97-4E9D-B186-1ABC21F6144C}"/>
+    <hyperlink ref="J26" r:id="rId54" tooltip="Supplier" display="'296-34818-6-ND" xr:uid="{80687301-253A-4487-830A-ACAB4135DFD4}"/>
+    <hyperlink ref="J27" r:id="rId55" tooltip="Supplier" display="'296-21898-2-ND" xr:uid="{C690A03B-FCC0-4086-B2FE-8F2615814C97}"/>
   </hyperlinks>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.59055118110236227" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId56"/>
@@ -3586,13 +3586,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.5546875" customWidth="1"/>
+    <col min="2" max="2" width="110.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>8</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>10</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>11</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
fixed bottom silkscreen, generated gerbers
</commit_message>
<xml_diff>
--- a/_schematics/Project Outputs for EEG_circuit/BOM/Bill of Materials-EEG_circuit.xlsx
+++ b/_schematics/Project Outputs for EEG_circuit/BOM/Bill of Materials-EEG_circuit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6148270F-7AA4-4D1D-8CA3-BF6F817FFF98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C014CE96-6B86-47F6-9EF6-94FE79D4393C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="2840" windowWidth="6400" windowHeight="3470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -122,10 +122,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>2020-02-11</t>
-  </si>
-  <si>
-    <t>1:42:53 PM</t>
+    <t>2020-02-13</t>
+  </si>
+  <si>
+    <t>1:51:41 PM</t>
   </si>
   <si>
     <t>Bill of Materials For Project [EEG_circuit.PrjPcb] (No PCB Document Selected)</t>
@@ -440,7 +440,7 @@
     <t>60</t>
   </si>
   <si>
-    <t>2020-02-11 1:42:53 PM</t>
+    <t>2020-02-13 1:51:41 PM</t>
   </si>
   <si>
     <t>Bill of Materials</t>
@@ -2330,11 +2330,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>43872</v>
+        <v>43874</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>43872.571857986113</v>
+        <v>43874.577807175927</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="20"/>
@@ -2462,20 +2462,14 @@
       <c r="J11" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="38">
-        <v>1</v>
-      </c>
+      <c r="K11" s="38"/>
       <c r="L11" s="38">
-        <v>2217</v>
-      </c>
-      <c r="M11" s="76">
-        <v>1.19</v>
-      </c>
-      <c r="N11" s="76">
-        <v>1.19</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="104" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2512,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="37">
-        <v>2530</v>
+        <v>2505</v>
       </c>
       <c r="M12" s="75">
         <v>0.75</v>
@@ -2558,7 +2552,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="38">
-        <v>2581</v>
+        <v>2579</v>
       </c>
       <c r="M13" s="76">
         <v>0.54</v>
@@ -2828,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="38">
-        <v>136805</v>
+        <v>134140</v>
       </c>
       <c r="M19" s="76">
         <v>0.45</v>
@@ -2920,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="38">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="M21" s="76">
         <v>0.69</v>
@@ -2966,7 +2960,7 @@
         <v>2</v>
       </c>
       <c r="L22" s="37">
-        <v>69290</v>
+        <v>69240</v>
       </c>
       <c r="M22" s="75">
         <v>0.3</v>
@@ -3012,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="38">
-        <v>33012</v>
+        <v>33002</v>
       </c>
       <c r="M23" s="76">
         <v>0.41</v>
@@ -3150,7 +3144,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="37">
-        <v>1280</v>
+        <v>1265</v>
       </c>
       <c r="M26" s="75">
         <v>53.84</v>
@@ -3218,13 +3212,13 @@
       <c r="J28" s="39"/>
       <c r="K28" s="43">
         <f>SUM(K10:K27)</f>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L28" s="42"/>
       <c r="M28" s="42"/>
       <c r="N28" s="42">
         <f>SUM(N10:N27)</f>
-        <v>67.77000000000001</v>
+        <v>66.58</v>
       </c>
       <c r="O28" s="62"/>
     </row>
@@ -3269,7 +3263,7 @@
       <c r="K30" s="36"/>
       <c r="L30" s="78">
         <f>N28</f>
-        <v>67.77000000000001</v>
+        <v>66.58</v>
       </c>
       <c r="M30" s="79"/>
       <c r="N30" s="89" t="s">
@@ -3293,7 +3287,7 @@
       <c r="K31" s="6"/>
       <c r="L31" s="80">
         <f>L30/H30</f>
-        <v>67.77000000000001</v>
+        <v>66.58</v>
       </c>
       <c r="M31" s="80"/>
       <c r="N31" s="90" t="s">
@@ -3512,60 +3506,60 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D10" r:id="rId2" tooltip="Component" display="'JST" xr:uid="{E17CCF0C-CA77-4AF2-AC5B-80A8951316D4}"/>
-    <hyperlink ref="D11" r:id="rId3" tooltip="Component" display="'Global Connector Technology" xr:uid="{8AD69FE7-D361-4A06-8B5D-58220CAE4C48}"/>
-    <hyperlink ref="D12" r:id="rId4" tooltip="Component" display="'Wurth Electronics" xr:uid="{821447E0-395D-447C-B3F0-786D1C72C06C}"/>
-    <hyperlink ref="D13" r:id="rId5" tooltip="Component" display="'Wurth Electronics" xr:uid="{F0F42E58-5414-4872-8D42-CDABAEF31BAF}"/>
-    <hyperlink ref="D14" r:id="rId6" tooltip="Component" display="'Wurth Electronics" xr:uid="{16D82F29-F51E-4BCE-A73E-D291925847FB}"/>
-    <hyperlink ref="D15" r:id="rId7" tooltip="Component" display="'Panasonic" xr:uid="{994E6F34-49CE-4442-9B91-844E590CCE3F}"/>
-    <hyperlink ref="D16" r:id="rId8" tooltip="Component" display="'Yageo" xr:uid="{9EEA62B6-FD2C-4591-8DB8-B9AC15816F20}"/>
-    <hyperlink ref="D17" r:id="rId9" tooltip="Component" display="'Murata, Samsung, KEMET" xr:uid="{AC4D51EB-6330-47A9-85E2-F2C866DD3B46}"/>
-    <hyperlink ref="D18" r:id="rId10" tooltip="Component" display="'TDK" xr:uid="{E93501FA-C544-465E-8376-435256E848E3}"/>
-    <hyperlink ref="D19" r:id="rId11" tooltip="Component" display="'Vishay Lite-On" xr:uid="{7A671E01-2B06-4F3E-B243-47F2A70C2282}"/>
-    <hyperlink ref="D20" r:id="rId12" tooltip="Component" display="'Yageo" xr:uid="{2364ED70-3793-4940-B3A6-E9380E02ECED}"/>
-    <hyperlink ref="D21" r:id="rId13" tooltip="Component" display="'ECS International" xr:uid="{6027C9AA-A15B-4F31-A5BE-A3C38C5CDF6B}"/>
-    <hyperlink ref="D22" r:id="rId14" tooltip="Component" display="'ITT C&amp;K" xr:uid="{802C777E-E8C0-4B9B-99A5-B9C133ABF11E}"/>
-    <hyperlink ref="D23" r:id="rId15" tooltip="Component" display="'Diodes" xr:uid="{E681CCC8-B3B8-4E5B-9052-DA8AB41B9FB8}"/>
-    <hyperlink ref="D24" r:id="rId16" tooltip="Component" display="'Microchip" xr:uid="{EB27A58A-2076-4830-8122-635583F22CDC}"/>
-    <hyperlink ref="D25" r:id="rId17" tooltip="Component" display="'Vishay Semiconductors" xr:uid="{8CBE7A95-84B7-4B4C-8980-FFBA63433157}"/>
-    <hyperlink ref="D26" r:id="rId18" tooltip="Component" display="'Texas Instruments" xr:uid="{3EDBDE57-5D16-4116-B073-CAB1D5E12CE3}"/>
-    <hyperlink ref="D27" r:id="rId19" tooltip="Component" display="'Texas Instruments" xr:uid="{AB61C659-5E4A-4E7F-8091-A0C1C8A98685}"/>
-    <hyperlink ref="E10" r:id="rId20" tooltip="Manufacturer" display="'B2B-PH-SM4-TBT(LF)(SN)" xr:uid="{C398540D-2562-4D55-8B25-69F89142FD02}"/>
-    <hyperlink ref="E11" r:id="rId21" tooltip="Manufacturer" display="'MEM2067-02-180-00-A" xr:uid="{05FF8958-9B7D-403C-89E7-831A1FF967FE}"/>
-    <hyperlink ref="E12" r:id="rId22" tooltip="Manufacturer" display="'450404015514" xr:uid="{C6AA90D6-775A-40A6-BF1C-2942D5E6BAC3}"/>
-    <hyperlink ref="E13" r:id="rId23" tooltip="Manufacturer" display="'61300621121" xr:uid="{E46A51EF-0CD3-4D0E-B11C-04CD6F3B27D7}"/>
-    <hyperlink ref="E14" r:id="rId24" tooltip="Manufacturer" display="'61301211121" xr:uid="{4126F58B-64EB-48E9-ADA3-53E87A432258}"/>
-    <hyperlink ref="E15" r:id="rId25" tooltip="Manufacturer" display="'EXB-N8V162JX" xr:uid="{851C9639-2AA7-4051-AD7C-9A846F6278FE}"/>
-    <hyperlink ref="E16" r:id="rId26" tooltip="Manufacturer" display="'RC0402FR-071ML, RC0402JR-070RL, RC0402FR-07453KL, RC0402FR-07100KL, RC0402JR-071M6L, RC0402JR-07180KL, RC0402FR-0710KL, RC0402FR-071KL, RC0402JR-07470KL" xr:uid="{66CFB7AA-0BAB-4440-9E47-2DE073582567}"/>
-    <hyperlink ref="E17" r:id="rId27" tooltip="Manufacturer" display="'GRM153R61A105ME95D, CL05A104KP5NNNC, CL05B152KB5NNNC, GRM155R61A475MEAAD, CL05A106MP5NUNC, GRM31CR60J107ME39L, C0402C180K5RAC7867" xr:uid="{7B70886D-5D47-4155-862F-114A40059966}"/>
-    <hyperlink ref="E18" r:id="rId28" tooltip="Manufacturer" display="'MLZ1608A2R2WT000, MLZ1608M4R7WT000" xr:uid="{DAAED366-F176-4783-8CFF-43FD9E11AA20}"/>
-    <hyperlink ref="E19" r:id="rId29" tooltip="Manufacturer" display="'LTST-C193TBKT-5A" xr:uid="{9DE918CC-D989-4B79-95F4-D12F6AC24A03}"/>
-    <hyperlink ref="E20" r:id="rId30" tooltip="Manufacturer" display="'CA0612KRX7R9BB102" xr:uid="{61B81365-FDA8-488A-87FC-0DCFE4CF8AAB}"/>
-    <hyperlink ref="E21" r:id="rId31" tooltip="Manufacturer" display="'ECS-80-18-30-JGN-TR" xr:uid="{ABD2BEFF-A50F-4DE1-9A40-C0E80D0D0B85}"/>
-    <hyperlink ref="E22" r:id="rId32" tooltip="Manufacturer" display="'PTS810SJK250SMTRLFS" xr:uid="{28CD9B91-DAAD-469F-9D31-2215DBBF2763}"/>
-    <hyperlink ref="E23" r:id="rId33" tooltip="Manufacturer" display="'AP3417CKTR-G1" xr:uid="{8AF274D8-87EE-46AB-8E52-0B9F7033901E}"/>
-    <hyperlink ref="E24" r:id="rId34" tooltip="Manufacturer" display="'PIC32MX250F128B-I/SS" xr:uid="{27C7DF5D-0D4A-4C31-ACA8-E4F4FC12EB99}"/>
-    <hyperlink ref="E25" r:id="rId35" tooltip="Manufacturer" display="'GSOT04C-G3-08" xr:uid="{490F205B-33CF-4390-896C-147AF756FE1E}"/>
-    <hyperlink ref="E26" r:id="rId36" tooltip="Manufacturer" display="'ADS1299IPAGR" xr:uid="{E1146058-33FF-4048-BCB6-4A64824CDCC4}"/>
-    <hyperlink ref="E27" r:id="rId37" tooltip="Manufacturer" display="'TPS61073DDCR" xr:uid="{39446364-C491-4226-B9C7-FD1CD60DE094}"/>
-    <hyperlink ref="J10" r:id="rId38" tooltip="Supplier" display="'455-2872-6-ND" xr:uid="{4D0A465C-FAA5-4639-A6E5-2630AFA5906F}"/>
-    <hyperlink ref="J11" r:id="rId39" tooltip="Supplier" display="'2073-MEM2067-02-180-00-ACT-ND" xr:uid="{CF1B3474-8070-409E-AE77-372DEBD666CB}"/>
-    <hyperlink ref="J12" r:id="rId40" tooltip="Supplier" display="'732-13665-6-ND" xr:uid="{62161FBE-5A25-4BD4-8BB8-838F78D0145A}"/>
-    <hyperlink ref="J13" r:id="rId41" tooltip="Supplier" display="'732-5295-ND" xr:uid="{8E9AF0C5-F08B-4DC0-8B33-58852FCD6F63}"/>
-    <hyperlink ref="J14" r:id="rId42" tooltip="Supplier" display="'732-5323-ND" xr:uid="{0232E260-FF16-49E6-94D2-3EE612F3884B}"/>
-    <hyperlink ref="J15" r:id="rId43" tooltip="Supplier" display="'Y10162DKR-ND" xr:uid="{319B4216-CE46-4571-80E9-4698BA7B9000}"/>
-    <hyperlink ref="J16" r:id="rId44" tooltip="Supplier" display="'311-1.00MLRCT-ND, 311-0.0JRDKR-ND, YAG3164DKR-ND, 311-100KLRCT-ND, YAG3284DKR-ND, 311-180KJRDKR-ND, 311-10.0KLRDKR-ND, 311-1.00KLRDKR-ND, 311-470KJRDKR-ND" xr:uid="{B12550CE-B39B-4151-8E94-17794D27192F}"/>
-    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'490-14577-6-ND, 1276-1022-6-ND, 1276-1521-6-ND, 490-14306-6-ND, 1276-1450-6-ND, 490-4539-6-ND, 399-19371-6-ND" xr:uid="{B24B7F2B-AA0F-4145-9CB6-E9ACCAE3E0B1}"/>
-    <hyperlink ref="J18" r:id="rId46" tooltip="Supplier" display="'445-6385-6-ND, 445-6390-6-ND" xr:uid="{35DAEC10-9C18-4104-B3F4-B91E10C36CB5}"/>
-    <hyperlink ref="J19" r:id="rId47" tooltip="Supplier" display="'160-1827-1-ND" xr:uid="{7881D3C6-51DB-42B0-AEAE-197FAB418104}"/>
-    <hyperlink ref="J20" r:id="rId48" tooltip="Supplier" display="'311-2073-6-ND" xr:uid="{F1F67F2D-CC8B-4549-BDC9-8527F20B7A32}"/>
-    <hyperlink ref="J21" r:id="rId49" tooltip="Supplier" display="'XC2103DKR-ND" xr:uid="{03A34192-D2AC-4C9A-A1E6-721BA70C6D50}"/>
-    <hyperlink ref="J22" r:id="rId50" tooltip="Supplier" display="'CKN10503DKR-ND" xr:uid="{D929463E-86F6-40C8-8D0F-114B511E46E4}"/>
-    <hyperlink ref="J23" r:id="rId51" tooltip="Supplier" display="'AP3417CKTR-G1DIDKR-ND" xr:uid="{98E19703-1CE9-4F9E-A3A3-5ADD5EC75BB6}"/>
-    <hyperlink ref="J24" r:id="rId52" tooltip="Supplier" display="'PIC32MX250F128B-I/SS-ND" xr:uid="{77972A37-6726-42E0-B48B-92AB90F2FFDA}"/>
-    <hyperlink ref="J25" r:id="rId53" tooltip="Supplier" display="'GSOT04C-G3-08GIDKR-ND" xr:uid="{B3E61186-8A97-4E9D-B186-1ABC21F6144C}"/>
-    <hyperlink ref="J26" r:id="rId54" tooltip="Supplier" display="'296-34818-6-ND" xr:uid="{80687301-253A-4487-830A-ACAB4135DFD4}"/>
-    <hyperlink ref="J27" r:id="rId55" tooltip="Supplier" display="'296-21898-2-ND" xr:uid="{C690A03B-FCC0-4086-B2FE-8F2615814C97}"/>
+    <hyperlink ref="D10" r:id="rId2" tooltip="Component" display="'JST" xr:uid="{7414E2C8-641D-43D7-B80F-A3E591188267}"/>
+    <hyperlink ref="D11" r:id="rId3" tooltip="Component" display="'Global Connector Technology" xr:uid="{18D8D976-40AA-4E61-AE50-1F157EA53D02}"/>
+    <hyperlink ref="D12" r:id="rId4" tooltip="Component" display="'Wurth Electronics" xr:uid="{D1AFBA61-728E-4F2F-8C34-9A139845FEC4}"/>
+    <hyperlink ref="D13" r:id="rId5" tooltip="Component" display="'Wurth Electronics" xr:uid="{053BCAFE-A57E-4AE3-880B-8C2AAE7D9BC4}"/>
+    <hyperlink ref="D14" r:id="rId6" tooltip="Component" display="'Wurth Electronics" xr:uid="{06485DA6-B175-4899-B7ED-72990E3376A3}"/>
+    <hyperlink ref="D15" r:id="rId7" tooltip="Component" display="'Panasonic" xr:uid="{AFAB0DBE-E02F-4EDE-AFCB-171ADE22B00A}"/>
+    <hyperlink ref="D16" r:id="rId8" tooltip="Component" display="'Yageo" xr:uid="{F5C04F83-EFB7-41C3-B283-28F0241DE94E}"/>
+    <hyperlink ref="D17" r:id="rId9" tooltip="Component" display="'Murata, Samsung, KEMET" xr:uid="{FC8CAEE3-160F-4B27-BD4F-7846AF352F33}"/>
+    <hyperlink ref="D18" r:id="rId10" tooltip="Component" display="'TDK" xr:uid="{B6FBB7E7-56BB-43EC-BC40-C9DCC3E07DD1}"/>
+    <hyperlink ref="D19" r:id="rId11" tooltip="Component" display="'Vishay Lite-On" xr:uid="{513A9F79-82E3-4993-8F12-A853698D58D8}"/>
+    <hyperlink ref="D20" r:id="rId12" tooltip="Component" display="'Yageo" xr:uid="{D5B97504-7271-4AB7-A5DE-419D961675C0}"/>
+    <hyperlink ref="D21" r:id="rId13" tooltip="Component" display="'ECS International" xr:uid="{01D31302-CBDF-4235-B4FB-B82C94142CE5}"/>
+    <hyperlink ref="D22" r:id="rId14" tooltip="Component" display="'ITT C&amp;K" xr:uid="{9C431BB5-D298-47F4-871F-CEE9A041C114}"/>
+    <hyperlink ref="D23" r:id="rId15" tooltip="Component" display="'Diodes" xr:uid="{11C70371-E322-4E5C-9F1D-CE06F5691AAF}"/>
+    <hyperlink ref="D24" r:id="rId16" tooltip="Component" display="'Microchip" xr:uid="{5DFAA53B-A98B-43F4-A760-18C93191431D}"/>
+    <hyperlink ref="D25" r:id="rId17" tooltip="Component" display="'Vishay Semiconductors" xr:uid="{FD3E4C9B-2C94-4853-8F5C-1604E7F9AA97}"/>
+    <hyperlink ref="D26" r:id="rId18" tooltip="Component" display="'Texas Instruments" xr:uid="{D104A672-A8FE-49AD-9F5E-7267337682A1}"/>
+    <hyperlink ref="D27" r:id="rId19" tooltip="Component" display="'Texas Instruments" xr:uid="{EB19F061-6F56-41B2-BF62-648759B6702C}"/>
+    <hyperlink ref="E10" r:id="rId20" tooltip="Manufacturer" display="'B2B-PH-SM4-TBT(LF)(SN)" xr:uid="{A10B1DAF-CCB8-4D95-9212-AA22B07B7B63}"/>
+    <hyperlink ref="E11" r:id="rId21" tooltip="Manufacturer" display="'MEM2067-02-180-00-A" xr:uid="{8C060D02-103F-46FD-B8B1-4DECA93670D8}"/>
+    <hyperlink ref="E12" r:id="rId22" tooltip="Manufacturer" display="'450404015514" xr:uid="{4F287346-19C3-48D6-B128-A83A85E774C0}"/>
+    <hyperlink ref="E13" r:id="rId23" tooltip="Manufacturer" display="'61300621121" xr:uid="{B69911E7-4B72-468E-8344-A73B156E7603}"/>
+    <hyperlink ref="E14" r:id="rId24" tooltip="Manufacturer" display="'61301211121" xr:uid="{5C9B4C38-AE5D-4F98-91C3-8EEFDEEB6460}"/>
+    <hyperlink ref="E15" r:id="rId25" tooltip="Manufacturer" display="'EXB-N8V162JX" xr:uid="{84592B44-570B-419C-B633-E21A0832BB4A}"/>
+    <hyperlink ref="E16" r:id="rId26" tooltip="Manufacturer" display="'RC0402FR-071ML, RC0402JR-070RL, RC0402FR-07453KL, RC0402FR-07100KL, RC0402JR-071M6L, RC0402JR-07180KL, RC0402FR-0710KL, RC0402FR-071KL, RC0402JR-07470KL" xr:uid="{10070596-FF97-41C9-8D47-2BD439B96DB5}"/>
+    <hyperlink ref="E17" r:id="rId27" tooltip="Manufacturer" display="'GRM153R61A105ME95D, CL05A104KP5NNNC, CL05B152KB5NNNC, GRM155R61A475MEAAD, CL05A106MP5NUNC, GRM31CR60J107ME39L, C0402C180K5RAC7867" xr:uid="{DB5D88D1-D176-4442-980D-E5F2BDE5DAC0}"/>
+    <hyperlink ref="E18" r:id="rId28" tooltip="Manufacturer" display="'MLZ1608A2R2WT000, MLZ1608M4R7WT000" xr:uid="{52E5FD3C-A3F3-4308-A4D1-4E4136B632CF}"/>
+    <hyperlink ref="E19" r:id="rId29" tooltip="Manufacturer" display="'LTST-C193TBKT-5A" xr:uid="{A360BB26-2A87-4003-9FF4-ACABDCE37D17}"/>
+    <hyperlink ref="E20" r:id="rId30" tooltip="Manufacturer" display="'CA0612KRX7R9BB102" xr:uid="{ECC1BC6B-5921-4AE6-BD68-209BF1546CA1}"/>
+    <hyperlink ref="E21" r:id="rId31" tooltip="Manufacturer" display="'ECS-80-18-30-JGN-TR" xr:uid="{4F33D2E5-C482-447A-865F-A65778769E20}"/>
+    <hyperlink ref="E22" r:id="rId32" tooltip="Manufacturer" display="'PTS810SJK250SMTRLFS" xr:uid="{0EA70310-6719-4072-86DA-35720D2B4A5B}"/>
+    <hyperlink ref="E23" r:id="rId33" tooltip="Manufacturer" display="'AP3417CKTR-G1" xr:uid="{9549E058-3F54-4AA8-8BD0-9EDAB1EEA448}"/>
+    <hyperlink ref="E24" r:id="rId34" tooltip="Manufacturer" display="'PIC32MX250F128B-I/SS" xr:uid="{4AB39837-9492-4CE9-903F-D7016FE91E1B}"/>
+    <hyperlink ref="E25" r:id="rId35" tooltip="Manufacturer" display="'GSOT04C-G3-08" xr:uid="{AB25CFCF-4EE3-4CDD-B192-C866422E74F5}"/>
+    <hyperlink ref="E26" r:id="rId36" tooltip="Manufacturer" display="'ADS1299IPAGR" xr:uid="{D697F671-E7D0-4040-8941-D13C07CE5513}"/>
+    <hyperlink ref="E27" r:id="rId37" tooltip="Manufacturer" display="'TPS61073DDCR" xr:uid="{1C9CC195-D432-461C-A376-9D0FAE257B90}"/>
+    <hyperlink ref="J10" r:id="rId38" tooltip="Supplier" display="'455-2872-6-ND" xr:uid="{4DC43CB3-202C-4F8B-99D1-ECB84C67234C}"/>
+    <hyperlink ref="J11" r:id="rId39" tooltip="Supplier" display="'2073-MEM2067-02-180-00-ACT-ND" xr:uid="{B1DAA39C-A70C-4BD9-9ECD-2A2225089538}"/>
+    <hyperlink ref="J12" r:id="rId40" tooltip="Supplier" display="'732-13665-6-ND" xr:uid="{4F6A3FE2-58D8-479D-A73D-04D88D62355C}"/>
+    <hyperlink ref="J13" r:id="rId41" tooltip="Supplier" display="'732-5295-ND" xr:uid="{A118AD8F-0EA3-4AAD-9322-19E631D09917}"/>
+    <hyperlink ref="J14" r:id="rId42" tooltip="Supplier" display="'732-5323-ND" xr:uid="{BA66526A-B3BF-400E-A542-4AD9F67C1677}"/>
+    <hyperlink ref="J15" r:id="rId43" tooltip="Supplier" display="'Y10162DKR-ND" xr:uid="{D8C03F3F-0D4C-4E7A-B5AC-124D0C2954BF}"/>
+    <hyperlink ref="J16" r:id="rId44" tooltip="Supplier" display="'311-1.00MLRCT-ND, 311-0.0JRDKR-ND, YAG3164DKR-ND, 311-100KLRCT-ND, YAG3284DKR-ND, 311-180KJRDKR-ND, 311-10.0KLRDKR-ND, 311-1.00KLRDKR-ND, 311-470KJRDKR-ND" xr:uid="{3C561A05-1609-47A0-928A-EA65452823B6}"/>
+    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'490-14577-6-ND, 1276-1022-6-ND, 1276-1521-6-ND, 490-14306-6-ND, 1276-1450-6-ND, 490-4539-6-ND, 399-19371-6-ND" xr:uid="{822A4AC3-3CFD-46E2-AC64-D5CE21CABCD0}"/>
+    <hyperlink ref="J18" r:id="rId46" tooltip="Supplier" display="'445-6385-6-ND, 445-6390-6-ND" xr:uid="{519B7A65-7784-410F-8E2C-165C30F3895D}"/>
+    <hyperlink ref="J19" r:id="rId47" tooltip="Supplier" display="'160-1827-1-ND" xr:uid="{198EDFB5-E50C-4482-BB68-ACF834C9E514}"/>
+    <hyperlink ref="J20" r:id="rId48" tooltip="Supplier" display="'311-2073-6-ND" xr:uid="{AE3313BE-9571-41C5-A85D-CD4BF15652F9}"/>
+    <hyperlink ref="J21" r:id="rId49" tooltip="Supplier" display="'XC2103DKR-ND" xr:uid="{107B4232-EED4-49E8-A878-C7820082D394}"/>
+    <hyperlink ref="J22" r:id="rId50" tooltip="Supplier" display="'CKN10503DKR-ND" xr:uid="{61C3E51F-B33B-469B-948E-1744062C4387}"/>
+    <hyperlink ref="J23" r:id="rId51" tooltip="Supplier" display="'AP3417CKTR-G1DIDKR-ND" xr:uid="{5E44CAEF-2D6F-4A3E-A91B-CAB3886D3C9F}"/>
+    <hyperlink ref="J24" r:id="rId52" tooltip="Supplier" display="'PIC32MX250F128B-I/SS-ND" xr:uid="{068A219C-AECC-4F63-9480-8FB143801E5E}"/>
+    <hyperlink ref="J25" r:id="rId53" tooltip="Supplier" display="'GSOT04C-G3-08GIDKR-ND" xr:uid="{D2C38072-70B9-4F79-9D21-849762744265}"/>
+    <hyperlink ref="J26" r:id="rId54" tooltip="Supplier" display="'296-34818-6-ND" xr:uid="{A988AE35-AD14-4F63-B644-C9A9D0504C0E}"/>
+    <hyperlink ref="J27" r:id="rId55" tooltip="Supplier" display="'296-21898-2-ND" xr:uid="{4B291EE5-42A8-4D32-88E0-07A524E642A6}"/>
   </hyperlinks>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.59055118110236227" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId56"/>
@@ -3656,7 +3650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>8</v>
       </c>
@@ -3664,7 +3658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3672,7 +3666,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>10</v>
       </c>
@@ -3680,7 +3674,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>11</v>
       </c>
@@ -3688,7 +3682,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
@@ -3696,7 +3690,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>13</v>
       </c>

</xml_diff>